<commit_message>
04/13/23 AC final edits for written report
</commit_message>
<xml_diff>
--- a/output/files/TripCt_Summary.xlsx
+++ b/output/files/TripCt_Summary.xlsx
@@ -549,10 +549,10 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>3614.63023812421</v>
+        <v>3736.72709330646</v>
       </c>
       <c r="C2" t="n">
-        <v>2929834</v>
+        <v>2926033</v>
       </c>
     </row>
     <row r="3">
@@ -560,10 +560,10 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>5051.29223387055</v>
+        <v>5223.53644314869</v>
       </c>
       <c r="C3" t="n">
-        <v>3183004</v>
+        <v>3179840</v>
       </c>
     </row>
     <row r="4">
@@ -571,10 +571,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>41661.2534501643</v>
+        <v>43068.5287981859</v>
       </c>
       <c r="C4" t="n">
-        <v>6244028</v>
+        <v>6235918</v>
       </c>
     </row>
     <row r="5">
@@ -582,10 +582,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>906.348683270632</v>
+        <v>936.86658286503</v>
       </c>
       <c r="C5" t="n">
-        <v>1250631</v>
+        <v>1248880</v>
       </c>
     </row>
   </sheetData>

</xml_diff>